<commit_message>
Skeleton of the project: with main functions
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -378,435 +378,1824 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>222</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>5</v>
       </c>
       <c r="D1">
-        <v>876042340</v>
+        <v>882141306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>210</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>891035994</v>
+        <v>874791623</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>224</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>888104457</v>
+        <v>879467936</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>303</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>785</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>879485318</v>
+        <v>889555384</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>387</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>879270459</v>
+        <v>885547314</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>274</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>879539794</v>
+        <v>882373865</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>291</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>1042</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>874834944</v>
+        <v>886031634</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1184</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
-        <v>892079237</v>
+        <v>887611649</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>392</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>886176814</v>
+        <v>882397146</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>167</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>486</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>892738452</v>
+        <v>874787497</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>299</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>877881320</v>
+        <v>879467260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>876973939</v>
+        <v>887745844</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>177</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>875537965</v>
+        <v>876699238</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>885412840</v>
+        <v>882376365</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>268</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>231</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>875744136</v>
+        <v>886030937</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>875636053</v>
+        <v>887427307</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>305</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>886324028</v>
+        <v>881515011</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>294</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>883612356</v>
+        <v>892078837</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>137</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>875975656</v>
+        <v>874791623</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>279</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>1336</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>875298353</v>
+        <v>879466547</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>790</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>660</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>885156904</v>
+        <v>885544911</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>424</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>880859722</v>
+        <v>893212929</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>864</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>775</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>888891473</v>
+        <v>882371645</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>782</v>
+        <v>9</v>
       </c>
       <c r="B24">
-        <v>1007</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>891500067</v>
+        <v>886030652</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="B25">
-        <v>678</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>889401432</v>
+        <v>887428060</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>861</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>949</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>881274937</v>
+        <v>882140037</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>782</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>1652</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>891500230</v>
+        <v>874787441</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>561</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>475</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28">
-        <v>885807393</v>
+        <v>879466457</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>363</v>
+        <v>5</v>
       </c>
       <c r="B29">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29">
-        <v>891496264</v>
+        <v>887745973</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>706</v>
+        <v>6</v>
       </c>
       <c r="B30">
-        <v>756</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D30">
-        <v>880997412</v>
+        <v>885544739</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>893212929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>882373656</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>887426931</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>882141485</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>892335920</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>874791960</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>879468307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>880889400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>885547360</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>886316140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>882396799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>886032204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>890887261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>882399357</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>892334267</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>874787549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>879468459</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>885545638</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>893213549</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>882396351</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>886031720</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>887426931</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>882140354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>892079373</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>874786488</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>887743141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>885547909</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>893213019</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>882372103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>886031437</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>881515296</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>892078936</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>874792483</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>879466937</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>885544881</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>893214128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>882371826</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>886031407</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>887473965</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>882140455</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>874792094</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>9</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>879466717</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>9</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>887747108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>6</v>
+      </c>
+      <c r="B74">
+        <v>9</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>885547124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>7</v>
+      </c>
+      <c r="B75">
+        <v>9</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75">
+        <v>893213918</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>8</v>
+      </c>
+      <c r="B76">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>887835408</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>9</v>
+      </c>
+      <c r="B77">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>886031912</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>10</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>888474646</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79">
+        <v>892079722</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>874791145</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>4</v>
+      </c>
+      <c r="B81">
+        <v>10</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>879467413</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>6</v>
+      </c>
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <v>885545263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="B83">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <v>893213644</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>8</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="D84">
+        <v>882396051</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>9</v>
+      </c>
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <v>886031342</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>10</v>
+      </c>
+      <c r="B86">
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>887472943</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>882139686</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88">
+        <v>11</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>892078890</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <v>874787496</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="B90">
+        <v>11</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <v>879466523</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>887745973</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>6</v>
+      </c>
+      <c r="B92">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>885545167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>7</v>
+      </c>
+      <c r="B93">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+      <c r="D93">
+        <v>893213549</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>8</v>
+      </c>
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="D94">
+        <v>882373531</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>9</v>
+      </c>
+      <c r="B95">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
+      </c>
+      <c r="D95">
+        <v>886030707</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>12</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>882397502</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>12</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>892335309</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>3</v>
+      </c>
+      <c r="B98">
+        <v>12</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>874792547</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>4</v>
+      </c>
+      <c r="B99">
+        <v>12</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>879467669</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>12</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>887746207</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>6</v>
+      </c>
+      <c r="B101">
+        <v>12</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>885547910</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <v>12</v>
+      </c>
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>882396489</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>886032098</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>10</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>887429669</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>13</v>
+      </c>
+      <c r="C105">
+        <v>5</v>
+      </c>
+      <c r="D105">
+        <v>882398814</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>13</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>892334079</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>5</v>
+      </c>
+      <c r="D107">
+        <v>874790926</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>4</v>
+      </c>
+      <c r="B108">
+        <v>13</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108">
+        <v>879483535</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>5</v>
+      </c>
+      <c r="B109">
+        <v>13</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+      <c r="D109">
+        <v>887746849</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>6</v>
+      </c>
+      <c r="B110">
+        <v>13</v>
+      </c>
+      <c r="C110">
+        <v>5</v>
+      </c>
+      <c r="D110">
+        <v>885545306</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <v>5</v>
+      </c>
+      <c r="D111">
+        <v>882371904</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>9</v>
+      </c>
+      <c r="B112">
+        <v>13</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>886030622</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>10</v>
+      </c>
+      <c r="B113">
+        <v>13</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+      <c r="D113">
+        <v>887693376</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>14</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+      <c r="D114">
+        <v>892334079</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
+      </c>
+      <c r="D115">
+        <v>874792692</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>4</v>
+      </c>
+      <c r="B116">
+        <v>14</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+      <c r="D116">
+        <v>879468459</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>6</v>
+      </c>
+      <c r="B117">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>4</v>
+      </c>
+      <c r="D117">
+        <v>885548330</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>7</v>
+      </c>
+      <c r="B118">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>5</v>
+      </c>
+      <c r="D118">
+        <v>893213549</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>8</v>
+      </c>
+      <c r="B119">
+        <v>14</v>
+      </c>
+      <c r="C119">
+        <v>4</v>
+      </c>
+      <c r="D119">
+        <v>882377861</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>9</v>
+      </c>
+      <c r="B120">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>3</v>
+      </c>
+      <c r="D120">
+        <v>886031752</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>10</v>
+      </c>
+      <c r="B121">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>4</v>
+      </c>
+      <c r="D121">
+        <v>887430102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>15</v>
+      </c>
+      <c r="C122">
+        <v>4</v>
+      </c>
+      <c r="D122">
+        <v>882397741</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="B123">
+        <v>15</v>
+      </c>
+      <c r="C123">
+        <v>4</v>
+      </c>
+      <c r="D123">
+        <v>874792574</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>15</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>879467607</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>5</v>
+      </c>
+      <c r="B125">
+        <v>15</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125">
+        <v>887746482</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>7</v>
+      </c>
+      <c r="B126">
+        <v>15</v>
+      </c>
+      <c r="C126">
+        <v>4</v>
+      </c>
+      <c r="D126">
+        <v>886317599</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>8</v>
+      </c>
+      <c r="B127">
+        <v>15</v>
+      </c>
+      <c r="C127">
+        <v>4</v>
+      </c>
+      <c r="D127">
+        <v>882473915</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>9</v>
+      </c>
+      <c r="B128">
+        <v>15</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>886032246</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>10</v>
+      </c>
+      <c r="B129">
+        <v>15</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>887611677</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:D150">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>